<commit_message>
Pushed all updates together
</commit_message>
<xml_diff>
--- a/scripts/IRIS_AIA.xlsx
+++ b/scripts/IRIS_AIA.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27b9ce8258b3956c/Desktop/aia/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{E0D8C48E-D852-494E-A44B-C2433999A6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE4F2B4-C382-44C1-A37D-24F02AFDDE68}"/>
+  <xr:revisionPtr revIDLastSave="452" documentId="13_ncr:1_{E0D8C48E-D852-494E-A44B-C2433999A6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A79087D8-0026-43FD-8A69-571324D25E02}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{2B3EA665-963F-4564-A132-85E31F0DA5E4}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="3" xr2:uid="{2B3EA665-963F-4564-A132-85E31F0DA5E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle4" sheetId="6" r:id="rId3"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId4"/>
+    <sheet name="test" sheetId="5" r:id="rId5"/>
+    <sheet name="Tabelle5" sheetId="7" r:id="rId6"/>
+    <sheet name="Comments" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="167">
   <si>
     <t>Event</t>
   </si>
@@ -297,157 +301,247 @@
     <t>2018-05-23T08:53:50</t>
   </si>
   <si>
-    <t xml:space="preserve">20130830_232946_4000257165 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20130902_163935_4000255147 </t>
-  </si>
-  <si>
-    <t>2013-08-30T23:29:46</t>
-  </si>
-  <si>
-    <t>2013-08-31T02:47:58</t>
-  </si>
-  <si>
-    <t>2013-09-02T16:39:35</t>
-  </si>
-  <si>
-    <t>2013-09-02T17:58:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20140618_045027_3863605388 </t>
-  </si>
-  <si>
-    <t>2014-06-18T04:50:27</t>
-  </si>
-  <si>
-    <t>2014-06-18T06:47:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20140620_232632_3863605388 </t>
-  </si>
-  <si>
-    <t>2014-06-20T23:26:32</t>
-  </si>
-  <si>
-    <t>2014-06-21T03:28:06</t>
-  </si>
-  <si>
     <t>2014-09-10T21:29:30</t>
   </si>
   <si>
     <t>2014-09-10T22:59:40</t>
   </si>
   <si>
+    <t>20141206_235804_3860100066</t>
+  </si>
+  <si>
+    <t>2014-12-06T23:58:04</t>
+  </si>
+  <si>
+    <t>2014-12-07T00:54:34</t>
+  </si>
+  <si>
+    <t>20150311_151947_3860107071</t>
+  </si>
+  <si>
+    <t>2015-03-11T15:19:47</t>
+  </si>
+  <si>
+    <t>2015-03-11T22:25:23</t>
+  </si>
+  <si>
+    <t>20150314_065918_3860605059</t>
+  </si>
+  <si>
+    <t>2015-03-14T06:59:18</t>
+  </si>
+  <si>
+    <t>2015-03-14T17:29:23</t>
+  </si>
+  <si>
+    <t>20150316_080555_3860607059</t>
+  </si>
+  <si>
+    <t>2015-03-16T08:05:54</t>
+  </si>
+  <si>
+    <t>2015-03-16T17:35:53</t>
+  </si>
+  <si>
+    <t>20150318_044701_3860107069</t>
+  </si>
+  <si>
+    <t>20150622_170003_3660100039</t>
+  </si>
+  <si>
+    <t>2015-06-22T17:00:03</t>
+  </si>
+  <si>
+    <t>2015-06-22T21:14:06</t>
+  </si>
+  <si>
+    <t>20150821_160115_3660104044</t>
+  </si>
+  <si>
+    <t>2015-08-21T16:01:15</t>
+  </si>
+  <si>
+    <t>2015-08-21T23:32:42</t>
+  </si>
+  <si>
+    <t>20151103_122743_3663600042</t>
+  </si>
+  <si>
+    <t>2015-11-03T12:27:43</t>
+  </si>
+  <si>
+    <t>2015-11-03T13:40:09</t>
+  </si>
+  <si>
+    <t>20151103_140515_3663600042</t>
+  </si>
+  <si>
+    <t>2015-11-03T14:05:15</t>
+  </si>
+  <si>
+    <t>2015-11-03T15:17:41</t>
+  </si>
+  <si>
+    <t>20160714_170018_3603105613</t>
+  </si>
+  <si>
+    <t>2016-07-14T17:00:18</t>
+  </si>
+  <si>
+    <t>2016-07-14T21:38:30</t>
+  </si>
+  <si>
     <t>20141027_140420_3860354980</t>
   </si>
   <si>
+    <t>20130830_232946_4000257165 2013-08-30T23:29:46.610 2013-08-31T02:47:58.475</t>
+  </si>
+  <si>
+    <t>20130902_163935_4000255147 2013-09-02T16:39:35.600 2013-09-02T17:58:48.385</t>
+  </si>
+  <si>
+    <t>20140618_045027_3863605388 2014-06-18T04:50:27.020 2014-06-18T06:47:03.954</t>
+  </si>
+  <si>
+    <t>20140620_232632_3863605388 2014-06-20T23:26:32.840 2014-06-21T03:28:06.264</t>
+  </si>
+  <si>
+    <t>20140910_212930_3800507454 2014-09-10T21:29:30.590 2014-09-10T22:59:40.882</t>
+  </si>
+  <si>
+    <t>20141027_140420_3860354980 2014-10-27T14:04:20.680 2014-10-27T17:44:56.632</t>
+  </si>
+  <si>
+    <t>20141204_181904_3800100083 2014-12-04T18:19:04.600 2014-12-04T19:15:57.163</t>
+  </si>
+  <si>
+    <t>20141206_235804_3860100066 2014-12-06T23:58:04.760 2014-12-07T00:54:34.411</t>
+  </si>
+  <si>
+    <t>20150311_151947_3860107071 2015-03-11T15:19:47.820 2015-03-11T22:25:23.174</t>
+  </si>
+  <si>
+    <t>20150314_065918_3860605059 2015-03-14T06:59:18.850 2015-03-14T17:29:23.543</t>
+  </si>
+  <si>
+    <t>20150316_080555_3860607059 2015-03-16T08:05:54.950 2015-03-16T17:35:53.543</t>
+  </si>
+  <si>
+    <t>20150318_044701_3860107069 2015-03-18T04:47:01.010 2015-03-19T02:47:25.268</t>
+  </si>
+  <si>
+    <t>20150622_170003_3660100039 2015-06-22T17:00:03.010 2015-06-22T21:14:06.632</t>
+  </si>
+  <si>
+    <t>20150821_160115_3660104044 2015-08-21T16:01:15.700 2015-08-21T23:32:42.522</t>
+  </si>
+  <si>
+    <t>20151103_122743_3663600042 2015-11-03T12:27:43.540 2015-11-03T13:40:09.528</t>
+  </si>
+  <si>
+    <t>20151103_140515_3663600042 2015-11-03T14:05:15.540 2015-11-03T15:17:41.528</t>
+  </si>
+  <si>
+    <t>20160714_170018_3603105613 2016-07-14T17:00:18.420 2016-07-14T21:38:30.360</t>
+  </si>
+  <si>
+    <t>20171005_074912_3645500435 2017-10-05T07:49:12.600 2017-10-05T11:00:25.718</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>Spalte2</t>
+  </si>
+  <si>
+    <t>Spalte3</t>
+  </si>
+  <si>
+    <t>Spalte4</t>
+  </si>
+  <si>
+    <t>Spalte5</t>
+  </si>
+  <si>
+    <t>Spalte6</t>
+  </si>
+  <si>
+    <t>Spalte7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obs </t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>20171005_074912_3645500435</t>
+  </si>
+  <si>
+    <t>2017-10-05T07:49:12.600</t>
+  </si>
+  <si>
+    <t>2017-10-05T11:00:25.718</t>
+  </si>
+  <si>
+    <t>20130830_232946_4000257165</t>
+  </si>
+  <si>
+    <t>2013-09-02T16:39:35.600</t>
+  </si>
+  <si>
+    <t>2013-09-02T17:58:48.385</t>
+  </si>
+  <si>
+    <t>2014-10-27T14:04:20.680</t>
+  </si>
+  <si>
+    <t>2014-10-27T17:44:56.632</t>
+  </si>
+  <si>
+    <t>2015-03-18T04:47:01.010</t>
+  </si>
+  <si>
+    <t>2015-03-19T02:47:25.268</t>
+  </si>
+  <si>
+    <t>2014-12-06T23:58:04.760</t>
+  </si>
+  <si>
+    <t>2014-12-07T00:54:34.411</t>
+  </si>
+  <si>
+    <t>2016-07-14T17:00:18.420</t>
+  </si>
+  <si>
+    <t>2016-07-14T21:38:30.360</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>plots</t>
+  </si>
+  <si>
+    <t>No data</t>
+  </si>
+  <si>
+    <t>Records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noisy , small flows </t>
+  </si>
+  <si>
+    <t>noisy</t>
+  </si>
+  <si>
+    <t>clear flows</t>
+  </si>
+  <si>
     <t>2014-10-27T14:04:20</t>
   </si>
   <si>
     <t>2014-10-27T17:44:56</t>
-  </si>
-  <si>
-    <t>20141206_235804_3860100066</t>
-  </si>
-  <si>
-    <t>2014-12-06T23:58:04</t>
-  </si>
-  <si>
-    <t>2014-12-07T00:54:34</t>
-  </si>
-  <si>
-    <t>20150311_151947_3860107071</t>
-  </si>
-  <si>
-    <t>2015-03-11T15:19:47</t>
-  </si>
-  <si>
-    <t>2015-03-11T22:25:23</t>
-  </si>
-  <si>
-    <t>20150314_065918_3860605059</t>
-  </si>
-  <si>
-    <t>2015-03-14T06:59:18</t>
-  </si>
-  <si>
-    <t>2015-03-14T17:29:23</t>
-  </si>
-  <si>
-    <t>20150316_080555_3860607059</t>
-  </si>
-  <si>
-    <t>2015-03-16T08:05:54</t>
-  </si>
-  <si>
-    <t>2015-03-16T17:35:53</t>
-  </si>
-  <si>
-    <t>20150318_044701_3860107069</t>
-  </si>
-  <si>
-    <t>2015-03-18T04:47:01</t>
-  </si>
-  <si>
-    <t>2015-03-19T02:47:25</t>
-  </si>
-  <si>
-    <t>20150622_170003_3660100039</t>
-  </si>
-  <si>
-    <t>2015-06-22T17:00:03</t>
-  </si>
-  <si>
-    <t>2015-06-22T21:14:06</t>
-  </si>
-  <si>
-    <t>20150821_160115_3660104044</t>
-  </si>
-  <si>
-    <t>2015-08-21T16:01:15</t>
-  </si>
-  <si>
-    <t>2015-08-21T23:32:42</t>
-  </si>
-  <si>
-    <t>20151103_122743_3663600042</t>
-  </si>
-  <si>
-    <t>2015-11-03T12:27:43</t>
-  </si>
-  <si>
-    <t>2015-11-03T13:40:09</t>
-  </si>
-  <si>
-    <t>20151103_140515_3663600042</t>
-  </si>
-  <si>
-    <t>2015-11-03T14:05:15</t>
-  </si>
-  <si>
-    <t>2015-11-03T15:17:41</t>
-  </si>
-  <si>
-    <t>20160714_170018_3603105613</t>
-  </si>
-  <si>
-    <t>2016-07-14T17:00:18</t>
-  </si>
-  <si>
-    <t>2016-07-14T21:38:30</t>
-  </si>
-  <si>
-    <t>20171005_074912_3645500435</t>
-  </si>
-  <si>
-    <t>2017-10-05T07:49:12</t>
-  </si>
-  <si>
-    <t>2017-10-05T11:00:25</t>
-  </si>
-  <si>
-    <t>No Si IV 1400</t>
   </si>
 </sst>
 </file>
@@ -457,7 +551,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +585,18 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="3"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -537,87 +643,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -660,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -708,94 +738,72 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -813,10 +821,38 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1110,13 +1146,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="6"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="6"/>
         </left>
@@ -1130,6 +1159,76 @@
           <color theme="6"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="6"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6"/>
+        </left>
+        <right style="thin">
+          <color theme="6"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1225,46 +1324,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{758D6AE3-D0A3-4822-90A1-0FE117938727}" name="Tabelle1" displayName="Tabelle1" ref="A1:E50" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{758D6AE3-D0A3-4822-90A1-0FE117938727}" name="Tabelle1" displayName="Tabelle1" ref="A1:E50" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A1:E50" xr:uid="{758D6AE3-D0A3-4822-90A1-0FE117938727}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AA3AFA23-97AD-46AC-88A7-A4AD26141B23}" name="Event" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{B38D9BC3-E62B-4F32-BDA0-DAAA200F7307}" name="X1" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{1B99999F-FC19-4216-BE1C-3839C2E76AA4}" name="Y1" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{8D0C2084-269E-4225-98A7-68B5D3B574A0}" name="X2" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{8103917A-9358-4948-A49E-3B63D3D290B7}" name="Y2" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{AA3AFA23-97AD-46AC-88A7-A4AD26141B23}" name="Event" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{B38D9BC3-E62B-4F32-BDA0-DAAA200F7307}" name="X1" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{1B99999F-FC19-4216-BE1C-3839C2E76AA4}" name="Y1" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{8D0C2084-269E-4225-98A7-68B5D3B574A0}" name="X2" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{8103917A-9358-4948-A49E-3B63D3D290B7}" name="Y2" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF8A9964-9C89-49A5-82DF-F7610ED6C1F1}" name="Tabelle13" displayName="Tabelle13" ref="A1:G33" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:G33" xr:uid="{CF8A9964-9C89-49A5-82DF-F7610ED6C1F1}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BD7337FA-EDF8-4712-AB03-F67C5B10D8A1}" name="Event" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{23A8C2CA-6E5A-4BD0-9732-D6C3214CD00E}" name="X1" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{3BAD4FF2-B090-4BFE-BF33-1D1E869F4B5E}" name="Y1" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{9C63DA04-7D6E-4D88-BF4B-AF997DCE41FD}" name="X2" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{871A5C96-97AD-4F1D-A44B-5EF781D766BF}" name="Y2" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7FD61C28-68B5-4E3C-BDC7-AE748DA028DE}" name="start_time" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{8988B5FF-5442-4F8A-9105-5A275D24B5CE}" name="end_time" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF8A9964-9C89-49A5-82DF-F7610ED6C1F1}" name="Tabelle13" displayName="Tabelle13" ref="A1:J26" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A1:J26" xr:uid="{CF8A9964-9C89-49A5-82DF-F7610ED6C1F1}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{BD7337FA-EDF8-4712-AB03-F67C5B10D8A1}" name="Event" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{23A8C2CA-6E5A-4BD0-9732-D6C3214CD00E}" name="X1" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{3BAD4FF2-B090-4BFE-BF33-1D1E869F4B5E}" name="Y1" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{9C63DA04-7D6E-4D88-BF4B-AF997DCE41FD}" name="X2" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{871A5C96-97AD-4F1D-A44B-5EF781D766BF}" name="Y2" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{7FD61C28-68B5-4E3C-BDC7-AE748DA028DE}" name="start_time" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{8988B5FF-5442-4F8A-9105-5A275D24B5CE}" name="end_time" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{2226A828-DFCA-4080-951D-3664EDD50C87}" name="plots" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{3CA8DBF5-4B26-4651-B8AA-C2F105BD261C}" name="Records" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{4A6A7DAC-99C9-498B-9FF4-4C58DB04B410}" name="Comments" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0B5A6A0A-6C76-42F0-9B05-507698ADEF8A}" name="Tabelle4" displayName="Tabelle4" ref="A1:G12" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:G12" xr:uid="{0B5A6A0A-6C76-42F0-9B05-507698ADEF8A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0B5A6A0A-6C76-42F0-9B05-507698ADEF8A}" name="Tabelle4" displayName="Tabelle4" ref="A1:G2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:G2" xr:uid="{0B5A6A0A-6C76-42F0-9B05-507698ADEF8A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{81FE55A4-8D1F-4DAE-A4B0-C869EE355A09}" name="Event" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{70AE6B3C-543A-4994-AE5B-5B7C46D0B999}" name="X1" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{B66FD642-E561-4F17-987B-53F333BD7DAE}" name="Y1" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{3250BA3F-2EEA-4355-AC0E-3769D5A8FAB4}" name="X2" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{DA242585-F33B-4E23-85A3-0DE471274786}" name="Y2" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{62346E38-688E-4B67-8DF8-B9897C8A469B}" name="start_time" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{0639E3CA-12E3-4F72-8C9F-E153322DD947}" name="end_time" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{81FE55A4-8D1F-4DAE-A4B0-C869EE355A09}" name="Event" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{70AE6B3C-543A-4994-AE5B-5B7C46D0B999}" name="X1" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B66FD642-E561-4F17-987B-53F333BD7DAE}" name="Y1" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{3250BA3F-2EEA-4355-AC0E-3769D5A8FAB4}" name="X2" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{DA242585-F33B-4E23-85A3-0DE471274786}" name="Y2" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{62346E38-688E-4B67-8DF8-B9897C8A469B}" name="start_time" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{0639E3CA-12E3-4F72-8C9F-E153322DD947}" name="end_time" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E56843D6-0132-451A-87B5-1D7D68898E04}" name="Tabelle5" displayName="Tabelle5" ref="A1:G7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:G7" xr:uid="{E56843D6-0132-451A-87B5-1D7D68898E04}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{7C462C1F-B936-4C88-9FD4-CBA66CE890E7}" name="Event" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{45E1377A-9888-47F9-B042-9274B21A3E33}" name="X1" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DAB6E8AB-D33B-4FD6-A91D-9FA20CAC4B3A}" name="Y1" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{31F75CD4-AC13-40EA-9E3F-AAA3E691F157}" name="X2" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{71647C3D-633B-4E38-B51A-60A1FF07B382}" name="Y2" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{0991855E-0359-48E8-8F7A-50B3B5B6670C}" name="start_time"/>
+    <tableColumn id="7" xr3:uid="{852AC6F3-3649-4316-A653-63485A31647E}" name="end_time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6A373F3E-FB6F-4F0B-8D7A-C3820E946845}" name="Tabelle3" displayName="Tabelle3" ref="A1:G22" totalsRowShown="0">
+  <autoFilter ref="A1:G22" xr:uid="{6A373F3E-FB6F-4F0B-8D7A-C3820E946845}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{4E9FBB26-23BD-4BD3-B0D8-62D0CCE7150E}" name="Spalte1"/>
+    <tableColumn id="2" xr3:uid="{41C5A2EB-17D8-4E4C-9F40-7AC6DE5AF37B}" name="Spalte2"/>
+    <tableColumn id="3" xr3:uid="{30414037-4652-4679-AEDE-CCB5F8A9DD16}" name="Spalte3"/>
+    <tableColumn id="4" xr3:uid="{A2E17A23-E228-4AEF-80BF-23642B75CF83}" name="Spalte4"/>
+    <tableColumn id="5" xr3:uid="{E2F8964A-D1D0-40BC-B68A-C401194BB878}" name="Spalte5"/>
+    <tableColumn id="6" xr3:uid="{4027CF8E-60ED-4367-84D7-96894FFB811E}" name="Spalte6"/>
+    <tableColumn id="7" xr3:uid="{8CF2189E-2200-4189-B964-DA012237E388}" name="Spalte7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3C174E61-5DD2-4B08-BE33-D61C53E246F3}" name="Tabelle6" displayName="Tabelle6" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{3C174E61-5DD2-4B08-BE33-D61C53E246F3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{EDEB021E-004B-4661-A3EC-EBCCC6430677}" name="Obs "/>
+    <tableColumn id="2" xr3:uid="{43C2335E-58D1-4EBC-BF32-2EC955521687}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1567,10 +1712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C44DE7F-2AA1-4F32-9F25-3675527D62F9}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2399,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2416,7 +2561,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -2433,7 +2578,53 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A51" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="10">
+        <v>1940</v>
+      </c>
+      <c r="C51" s="10">
+        <v>2007</v>
+      </c>
+      <c r="D51" s="10">
+        <v>1942</v>
+      </c>
+      <c r="E51" s="10">
+        <v>1720</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="2">
+        <v>3391</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2796</v>
+      </c>
+      <c r="D52" s="2">
+        <v>3395</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2509</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -2441,7 +2632,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -2460,10 +2651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20D6B51-FDBD-4712-B55C-B85C5D652CDA}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:G21"/>
+    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2471,9 +2662,11 @@
     <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.81640625" customWidth="1"/>
     <col min="6" max="7" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.2265625" customWidth="1"/>
+    <col min="10" max="10" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2495,13 +2688,22 @@
       <c r="G1" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>1938</v>
+        <v>1956</v>
       </c>
       <c r="C2" s="2">
         <v>2070</v>
@@ -2518,8 +2720,15 @@
       <c r="G2" s="13" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2541,8 +2750,15 @@
       <c r="G3" s="14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2558,14 +2774,21 @@
       <c r="E4" s="5">
         <v>2263</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2581,14 +2804,21 @@
       <c r="E5" s="5">
         <v>2510</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -2610,8 +2840,17 @@
       <c r="G6" s="15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2633,8 +2872,17 @@
       <c r="G7" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2656,8 +2904,17 @@
       <c r="G8" s="16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -2679,8 +2936,15 @@
       <c r="G9" s="14" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -2702,8 +2966,13 @@
       <c r="G10" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2725,8 +2994,13 @@
       <c r="G11" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -2748,8 +3022,13 @@
       <c r="G12" s="16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13" s="4" t="s">
         <v>49</v>
       </c>
@@ -2771,8 +3050,17 @@
       <c r="G13" s="14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2794,8 +3082,13 @@
       <c r="G14" s="16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -2817,8 +3110,13 @@
       <c r="G15" s="15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="H15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
@@ -2840,373 +3138,315 @@
       <c r="G16" s="16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A17" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1940</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2007</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1942</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1720</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="2">
-        <v>1271</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1963</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1272</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1880</v>
-      </c>
-      <c r="F17" s="16" t="s">
+      <c r="G17" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="B18" s="2">
+        <v>3391</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2796</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3395</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2509</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2218</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1989</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2219</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1889</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A19" s="17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="17">
+        <v>1476</v>
+      </c>
+      <c r="C19" s="17">
+        <v>2474</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1477</v>
+      </c>
+      <c r="E19" s="17">
+        <v>2279</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
+      <c r="G19" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A20" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="10">
+        <v>2344</v>
+      </c>
+      <c r="C20" s="10">
+        <v>2388</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2484</v>
+      </c>
+      <c r="E20" s="10">
+        <v>2252</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
+      <c r="G20" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="H20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A21" s="17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="10">
-        <v>1940</v>
-      </c>
-      <c r="C21" s="10">
-        <v>2007</v>
-      </c>
-      <c r="D21" s="10">
-        <v>1942</v>
-      </c>
-      <c r="E21" s="10">
-        <v>1720</v>
-      </c>
-      <c r="F21" s="10" t="s">
+      <c r="B21" s="17">
+        <v>2972</v>
+      </c>
+      <c r="C21" s="17">
+        <v>2436</v>
+      </c>
+      <c r="D21" s="17">
+        <v>3112</v>
+      </c>
+      <c r="E21" s="17">
+        <v>2300</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="17" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A22" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="s">
+      <c r="H21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A22" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="B22" s="17">
+        <v>2236</v>
+      </c>
+      <c r="C22" s="17">
+        <v>1797</v>
+      </c>
+      <c r="D22" s="17">
+        <v>2100</v>
+      </c>
+      <c r="E22" s="17">
+        <v>1658</v>
+      </c>
+      <c r="F22" s="17" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A23" s="2" t="s">
+      <c r="G22" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="2">
-        <v>3391</v>
-      </c>
-      <c r="C23" s="2">
-        <v>2796</v>
-      </c>
-      <c r="D23" s="2">
-        <v>3395</v>
-      </c>
-      <c r="E23" s="2">
-        <v>2509</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="H22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="B23" s="10">
+        <v>1279</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2654</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1281</v>
+      </c>
+      <c r="E23" s="10">
+        <v>2554</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A24" s="18" t="s">
+      <c r="G23" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B24" s="18">
-        <v>1476</v>
-      </c>
-      <c r="C24" s="18">
-        <v>2474</v>
-      </c>
-      <c r="D24" s="18">
-        <v>1477</v>
-      </c>
-      <c r="E24" s="18">
-        <v>2279</v>
-      </c>
-      <c r="F24" s="18" t="s">
+      <c r="H23" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A24" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="B24" s="17">
+        <v>1747</v>
+      </c>
+      <c r="C24" s="17">
+        <v>2045</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1748</v>
+      </c>
+      <c r="E24" s="17">
+        <v>1849</v>
+      </c>
+      <c r="F24" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G24" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A25" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B25" s="10">
-        <v>2344</v>
+        <v>1770</v>
       </c>
       <c r="C25" s="10">
-        <v>2388</v>
+        <v>2042</v>
       </c>
       <c r="D25" s="10">
-        <v>2484</v>
+        <v>1773</v>
       </c>
       <c r="E25" s="10">
-        <v>2252</v>
+        <v>1847</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A26" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="18">
-        <v>2972</v>
-      </c>
-      <c r="C26" s="18">
-        <v>2436</v>
-      </c>
-      <c r="D26" s="18">
-        <v>3112</v>
-      </c>
-      <c r="E26" s="18">
-        <v>2300</v>
-      </c>
-      <c r="F26" s="18" t="s">
+      <c r="H25" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A26" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="B26" s="17">
+        <v>1111</v>
+      </c>
+      <c r="C26" s="17">
+        <v>2112</v>
+      </c>
+      <c r="D26" s="17">
+        <v>1112</v>
+      </c>
+      <c r="E26" s="17">
+        <v>1918</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A27" s="10" t="s">
+      <c r="G26" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="10">
-        <v>3469</v>
-      </c>
-      <c r="C27" s="10">
-        <v>2617</v>
-      </c>
-      <c r="D27" s="10">
-        <v>3471</v>
-      </c>
-      <c r="E27" s="10">
-        <v>2329</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A28" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="18">
-        <v>2236</v>
-      </c>
-      <c r="C28" s="18">
-        <v>1797</v>
-      </c>
-      <c r="D28" s="18">
-        <v>2100</v>
-      </c>
-      <c r="E28" s="18">
-        <v>1658</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A29" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="10">
-        <v>1279</v>
-      </c>
-      <c r="C29" s="10">
-        <v>2654</v>
-      </c>
-      <c r="D29" s="10">
-        <v>1281</v>
-      </c>
-      <c r="E29" s="10">
-        <v>2554</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A30" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="18">
-        <v>1747</v>
-      </c>
-      <c r="C30" s="18">
-        <v>2045</v>
-      </c>
-      <c r="D30" s="18">
-        <v>1748</v>
-      </c>
-      <c r="E30" s="18">
-        <v>1849</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A31" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="10">
-        <v>1770</v>
-      </c>
-      <c r="C31" s="10">
-        <v>2042</v>
-      </c>
-      <c r="D31" s="10">
-        <v>1773</v>
-      </c>
-      <c r="E31" s="10">
-        <v>1847</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A32" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" s="18">
-        <v>1111</v>
-      </c>
-      <c r="C32" s="18">
-        <v>2112</v>
-      </c>
-      <c r="D32" s="18">
-        <v>1112</v>
-      </c>
-      <c r="E32" s="18">
-        <v>1918</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A33" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>135</v>
-      </c>
+      <c r="H26" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3219,299 +3459,415 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59410DDD-5582-47C7-A18F-366960084023}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F396548F-492E-40EA-93D2-81BD5D49048D}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1940</v>
-      </c>
-      <c r="C2" s="10">
-        <v>2007</v>
-      </c>
-      <c r="D2" s="10">
-        <v>1942</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1720</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="17">
-        <v>3391</v>
-      </c>
-      <c r="C3" s="17">
-        <v>2796</v>
-      </c>
-      <c r="D3" s="17">
-        <v>3395</v>
-      </c>
-      <c r="E3" s="17">
-        <v>2509</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A4" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="20">
-        <v>1476</v>
-      </c>
-      <c r="C4" s="20">
-        <v>2474</v>
-      </c>
-      <c r="D4" s="20">
-        <v>1477</v>
-      </c>
-      <c r="E4" s="20">
-        <v>2279</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A5" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="21">
-        <v>2344</v>
-      </c>
-      <c r="C5" s="21">
-        <v>2388</v>
-      </c>
-      <c r="D5" s="21">
-        <v>2484</v>
-      </c>
-      <c r="E5" s="21">
-        <v>2252</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A6" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="20">
-        <v>2972</v>
-      </c>
-      <c r="C6" s="20">
-        <v>2436</v>
-      </c>
-      <c r="D6" s="20">
-        <v>3112</v>
-      </c>
-      <c r="E6" s="20">
-        <v>2300</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A7" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="21">
-        <v>3469</v>
-      </c>
-      <c r="C7" s="21">
-        <v>2617</v>
-      </c>
-      <c r="D7" s="21">
-        <v>3471</v>
-      </c>
-      <c r="E7" s="21">
-        <v>2329</v>
-      </c>
-      <c r="F7" s="21" t="s">
+      <c r="A2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A8" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="20">
-        <v>2236</v>
-      </c>
-      <c r="C8" s="20">
-        <v>1797</v>
-      </c>
-      <c r="D8" s="20">
-        <v>2100</v>
-      </c>
-      <c r="E8" s="20">
-        <v>1658</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A9" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="21">
-        <v>1279</v>
-      </c>
-      <c r="C9" s="21">
-        <v>2654</v>
-      </c>
-      <c r="D9" s="21">
-        <v>1281</v>
-      </c>
-      <c r="E9" s="21">
-        <v>2554</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A10" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="20">
-        <v>1747</v>
-      </c>
-      <c r="C10" s="20">
-        <v>2045</v>
-      </c>
-      <c r="D10" s="20">
-        <v>1748</v>
-      </c>
-      <c r="E10" s="20">
-        <v>1849</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A11" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="21">
-        <v>1770</v>
-      </c>
-      <c r="C11" s="21">
-        <v>2042</v>
-      </c>
-      <c r="D11" s="21">
-        <v>1773</v>
-      </c>
-      <c r="E11" s="21">
-        <v>1847</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A12" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="29">
-        <v>1111</v>
-      </c>
-      <c r="C12" s="29">
-        <v>2112</v>
-      </c>
-      <c r="D12" s="29">
-        <v>1112</v>
-      </c>
-      <c r="E12" s="29">
-        <v>1918</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>132</v>
+      <c r="B2" s="9">
+        <v>3271</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2641</v>
+      </c>
+      <c r="D2" s="9">
+        <v>3273</v>
+      </c>
+      <c r="E2" s="9">
+        <v>2446</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9648D69-076A-4F94-8255-8924FB8069FB}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A5" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F85D0BC-42C5-472B-A9C6-0209A722F04A}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="105.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A2" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A3" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A4" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A5" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A6" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A7" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A8" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A9" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A10" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A11" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A12" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A13" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A14" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A15" s="22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A16" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A17" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A18" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18.25" x14ac:dyDescent="0.75">
+      <c r="A19" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4A825C-019E-4662-A29F-E0C77F7B83EC}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>